<commit_message>
Sector group selection fixed
</commit_message>
<xml_diff>
--- a/docs/Tasks.xlsx
+++ b/docs/Tasks.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC51D10-C4C9-4697-BBFC-92BC69A26B8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21957F87-E048-41C9-B15B-FC0EB9D81000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -41,9 +41,6 @@
     <t>DONE</t>
   </si>
   <si>
-    <t>TODO</t>
-  </si>
-  <si>
     <t xml:space="preserve">PRIORITÀ </t>
   </si>
   <si>
@@ -74,7 +71,16 @@
     <t>Dopo aver creato due room con ognuna 2 SG, se faccio picking su un SG di una stanza, passo all'altroa e provo a fare picking, ottengo una NullPointerException.</t>
   </si>
   <si>
-    <t>La selezione dei settori non funziona correttamente (passando da un SG all'altro, dovrebbe colorare di rosso quelli del SG corrente e, di bianco quelli relativi agli altri SG)</t>
+    <t>La selezione dei settori non funziona ancora (passando da un SG all'altro, dovrebbe colorare di rosso quelli del SG corrente e, di bianco quelli relativi agli altri SG)</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>IN PROGRESS</t>
+  </si>
+  <si>
+    <t>Passando da una room all'altra, se ruoto o faccio zoom su una sembra che anche l'altra (o le altre) tengono in memoria qualche trasformazione, invece dovrebbero essere indipendneti.</t>
   </si>
 </sst>
 </file>
@@ -186,7 +192,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -200,18 +206,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -223,6 +223,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -516,10 +519,10 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="H7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -528,7 +531,7 @@
     <col min="2" max="2" width="28" style="4" customWidth="1"/>
     <col min="3" max="3" width="9.81640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="39.453125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.81640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.7265625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="43.1796875" style="4" customWidth="1"/>
     <col min="7" max="7" width="11.54296875" style="2" customWidth="1"/>
     <col min="8" max="16384" width="8.7265625" style="4"/>
@@ -542,7 +545,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -554,7 +557,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
@@ -562,19 +565,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -582,137 +585,150 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="6"/>
       <c r="G4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
+        <v>7</v>
+      </c>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
     </row>
     <row r="5" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="A6" s="6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>16</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="7"/>
+      <c r="F6" s="6"/>
       <c r="G6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="7" t="s">
+      <c r="B7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="7"/>
+      <c r="D7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="6"/>
       <c r="G7" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="7"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="7"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="7"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>